<commit_message>
style PieChart inspired by the Mockup used for Twitter poll
</commit_message>
<xml_diff>
--- a/ios/Charts Libraries.xlsx
+++ b/ios/Charts Libraries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jan/workspace/mobsys22wise/ios/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9D6405F-52AD-E341-A02C-0943C6EF60F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24433E8E-C56B-8045-B01E-9D554DDD59D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="30720" windowHeight="17120" xr2:uid="{916433BB-9AC5-7948-874E-7EB1C28826DE}"/>
   </bookViews>
@@ -479,7 +479,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -488,6 +488,7 @@
     <col min="2" max="2" width="44.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="70.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -552,7 +553,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="121" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>

</xml_diff>